<commit_message>
fixed McCully in Imnaha
</commit_message>
<xml_diff>
--- a/data/USFWS_bull_trout_SSA_data_OR.xlsx
+++ b/data/USFWS_bull_trout_SSA_data_OR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheuerl/Documents/GitHub/bulltrout/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEAAEE0-FBE8-7647-8B82-4B36E4BD094F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DBF4F1-64EB-1F49-8191-ECFBB11DC7DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11760" yWindow="8640" windowWidth="23040" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10380" yWindow="1840" windowWidth="26740" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oregon Data" sheetId="1" r:id="rId1"/>
@@ -1102,9 +1102,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I647"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A469" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A481" sqref="A481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13574,9 +13574,6 @@
       </c>
     </row>
     <row r="481" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A481" s="14">
-        <v>21</v>
-      </c>
       <c r="B481" s="2" t="s">
         <v>32</v>
       </c>
@@ -18446,21 +18443,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056A396E11C201049A295728E554B4204" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5308e23870a69a858a1f647203e717c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e" xmlns:ns3="61093040-1240-489f-8ca6-d5903aeb7a38" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f096f016f089f4e04afada0be9633fb" ns2:_="" ns3:_="">
     <xsd:import namespace="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
@@ -18657,32 +18639,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E9542D-92F9-4D1A-958F-4A450E98A82B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="61093040-1240-489f-8ca6-d5903aeb7a38"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{596E4C84-42D4-4598-BDCF-3CCDF8B9CA62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{538184D0-EAB6-4E2D-9B7C-E6F8B2B1B871}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18699,4 +18671,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{596E4C84-42D4-4598-BDCF-3CCDF8B9CA62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E9542D-92F9-4D1A-958F-4A450E98A82B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="61093040-1240-489f-8ca6-d5903aeb7a38"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>